<commit_message>
Adding FF and Hotel membership code
</commit_message>
<xml_diff>
--- a/data/excel/ExpenseManagement.xlsx
+++ b/data/excel/ExpenseManagement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur.Yadav\git\ProjectQuadlabs\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\QuadlabsCoreProject\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9210DB08-5431-4B0A-8EEE-FBF05496DB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31A76E4-A836-459B-BD88-827D35DCCAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CF5A2F7A-4B78-411E-A600-51DCCD9C70AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="6" xr2:uid="{CF5A2F7A-4B78-411E-A600-51DCCD9C70AE}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpenseManagementReport" sheetId="31" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Reimbursement1" sheetId="35" r:id="rId4"/>
     <sheet name="ExpenseManagement" sheetId="28" r:id="rId5"/>
     <sheet name="Expensemanagement1" sheetId="33" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="36" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="201">
   <si>
     <t>Source</t>
   </si>
@@ -585,6 +586,63 @@
   </si>
   <si>
     <t>Report on Half Yearly Basis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCT Tour </t>
+  </si>
+  <si>
+    <t>23-Feb-2024</t>
+  </si>
+  <si>
+    <t>ExpenseFromDate</t>
+  </si>
+  <si>
+    <t>ExpenseToDate</t>
+  </si>
+  <si>
+    <t>26-Feb-2024</t>
+  </si>
+  <si>
+    <t>Conveyance</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>ConveyanceType</t>
+  </si>
+  <si>
+    <t>Taxi</t>
+  </si>
+  <si>
+    <t>Corigin</t>
+  </si>
+  <si>
+    <t>COrigin_Name</t>
+  </si>
+  <si>
+    <t>CDestination</t>
+  </si>
+  <si>
+    <t>CDestination_Name</t>
+  </si>
+  <si>
+    <t>del</t>
+  </si>
+  <si>
+    <t>bom</t>
+  </si>
+  <si>
+    <t>BombayMaharashtra, India</t>
+  </si>
+  <si>
+    <t>DelhiIndia</t>
+  </si>
+  <si>
+    <t>ConveyanceFromDate</t>
+  </si>
+  <si>
+    <t>ConveyanceToDate</t>
   </si>
 </sst>
 </file>
@@ -653,7 +711,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -676,12 +734,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -692,6 +761,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -711,9 +784,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -751,7 +824,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -857,7 +930,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -999,7 +1072,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1675,8 +1748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D15EE2C-CECE-42E2-A2DB-CBA1D6B4D6AA}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3570,8 +3643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4810EC-D59A-4293-94F2-3470C3C6AD5A}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4224,4 +4297,331 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2461470-3BD2-424D-B1B1-C1169DF2766B}">
+  <dimension ref="A1:AN2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AG13" sqref="AG13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="25" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:40" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="U2" s="1">
+        <v>500</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>6558864</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1500</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG2" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="AH2" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AM2" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations disablePrompts="1" count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2" xr:uid="{7E392B0E-D692-4A12-BBEF-49B320088420}">
+      <formula1>"Test117777 ( 222GHHHEEEYYY78 ),Chennai1 ( 22AAAHJUJJUJ9Z0 ),Chennai ( 22AAAHJUJJUJ9Z0 ),Mumbai Branch ( 22AAAHJUJJUJ9Z0 ),Delhi Branch ( 98526933 ),poonam corp1 (  )"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2" xr:uid="{25F2025E-D2E8-4C30-A037-9F7CAD1AD7D3}">
+      <formula1>"Entertainment,Expense,Flight,Fuel,Hotel,Meals,Other Product,Phone,Taxi,Transport"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2" xr:uid="{302B764B-13A0-4194-9E2A-31C5FB7BC893}">
+      <formula1>"Adjusted from Per Diem Account,Paid through Corporate Card,Adjust from Advances,Paid through Cash/Personal Card,Invoice to Company"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{71BCEA84-188D-419D-8463-28C966D550B8}">
+      <formula1>"Old Url,SSOLogin"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{489DC714-6F3F-4425-BAB7-1512CCAE2C81}">
+      <formula1>"laxmi.khanal@quadlabs.com,ankur.yadav@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2" xr:uid="{ED2140B8-2F80-48A5-BF68-F1633AF733F6}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH2" xr:uid="{AC352BE9-217F-4E84-A20C-0BCEBFE0F8BA}">
+      <formula1>"Taxi,Bike"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{17D67B72-6350-422D-8EAD-B1F8B59CE815}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>